<commit_message>
user order data fetched
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="103">
   <si>
     <t>SEM_EXM_EXCH_ID</t>
   </si>
@@ -167,34 +167,172 @@
     <t>OPTSTK</t>
   </si>
   <si>
-    <t>NAUKRI-Mar2025-9700-PE</t>
-  </si>
-  <si>
-    <t>NAUKRI 27 MAR 9700 PUT</t>
-  </si>
-  <si>
     <t>OP</t>
   </si>
   <si>
-    <t>NAUKRI-Apr2025-4000-CE</t>
-  </si>
-  <si>
-    <t>NAUKRI 24 APR 4000 CALL</t>
-  </si>
-  <si>
     <t>NAUKRI-Apr2025-4000-PE</t>
   </si>
   <si>
     <t>NAUKRI 24 APR 4000 PUT</t>
   </si>
   <si>
-    <t>hhh</t>
-  </si>
-  <si>
     <t>NAN-Apr2025-4400-CE</t>
   </si>
   <si>
     <t>NAN 24 APR 4400 CALL</t>
+  </si>
+  <si>
+    <t>AUBANK-Apr2025-585-PE</t>
+  </si>
+  <si>
+    <t>AUBANK 09 APR 585 PUT</t>
+  </si>
+  <si>
+    <t>AUSFOPT</t>
+  </si>
+  <si>
+    <t>IIFL-Mar2025-385-CE</t>
+  </si>
+  <si>
+    <t>IIFL 27 MAR 385 CALL</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-55-CE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 55 CALL</t>
+  </si>
+  <si>
+    <t>BHARATFORG-Mar2025-940-CE</t>
+  </si>
+  <si>
+    <t>BHARATFORG 27 MAR 940 CALL</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-55-PE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 55 PUT</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-65-CE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 65 CALL</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-65-PE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 65 PUT</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-72.5-CE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 72.50 CALL</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-72.5-PE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 72.50 PUT</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-77.5-CE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 77.50 CALL</t>
+  </si>
+  <si>
+    <t>IOC-Apr2025-77.5-PE</t>
+  </si>
+  <si>
+    <t>IOC 24 APR 77.50 PUT</t>
+  </si>
+  <si>
+    <t>ABB-Mar2025-7500-CE</t>
+  </si>
+  <si>
+    <t>ABB 27 MAR 7500 CALL</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>EQUITY</t>
+  </si>
+  <si>
+    <t>NIFTYIETF</t>
+  </si>
+  <si>
+    <t>ICICI Pru Nifty 50 ETF</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ETF</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Nifty ET</t>
+  </si>
+  <si>
+    <t>OPTIDX</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50-May2025-27000-PE</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50 29 MAY 27000 PUT</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50-May2025-27500-CE</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50 29 MAY 27500 CALL</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50-May2025-27500-PE</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50 29 MAY 27500 PUT</t>
+  </si>
+  <si>
+    <t>INDIGO-Mar2025-4800-CE</t>
+  </si>
+  <si>
+    <t>INDIGO 27 MAR 4800 CALL</t>
+  </si>
+  <si>
+    <t>INDIGO-Mar2025-4800-PE</t>
+  </si>
+  <si>
+    <t>INDIGO 27 MAR 4800 PUT</t>
+  </si>
+  <si>
+    <t>INDIGO-Apr2025-4650-PE</t>
+  </si>
+  <si>
+    <t>INDIGO 09 APR 4650 PUT</t>
+  </si>
+  <si>
+    <t>INALOPT</t>
+  </si>
+  <si>
+    <t>INDIGO-Apr2025-4800-CE</t>
+  </si>
+  <si>
+    <t>INDIGO 09 APR 4800 CALL</t>
+  </si>
+  <si>
+    <t>INDIGO-Apr2025-5100-PE</t>
+  </si>
+  <si>
+    <t>INDIGO 09 APR 5100 PUT</t>
   </si>
 </sst>
 </file>
@@ -513,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,95 +1051,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9">
-        <v>133977</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9">
-        <v>75</v>
-      </c>
-      <c r="H9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="1">
-        <v>45743.604166666664</v>
-      </c>
-      <c r="J9">
-        <v>9700</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9">
-        <v>5</v>
-      </c>
-      <c r="M9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" t="s">
-        <v>49</v>
-      </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10">
-        <v>133986</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10">
-        <v>75</v>
-      </c>
-      <c r="H10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="1">
-        <v>45771.604166666664</v>
-      </c>
-      <c r="J10">
-        <v>4000</v>
-      </c>
-      <c r="K10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10">
-        <v>5</v>
-      </c>
-      <c r="M10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" t="s">
-        <v>49</v>
-      </c>
-      <c r="P10" t="s">
-        <v>54</v>
-      </c>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1020,13 +1073,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G11">
         <v>75</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I11" s="1">
         <v>45771.604166666664</v>
@@ -1044,7 +1097,7 @@
         <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1064,13 +1117,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G12">
         <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1">
         <v>45771.604166666664</v>
@@ -1088,7 +1141,940 @@
         <v>22</v>
       </c>
       <c r="N12" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>852873</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="1">
+        <v>45756.645833333336</v>
+      </c>
+      <c r="J13">
+        <v>585</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>92647</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14">
+        <v>1550</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="1">
+        <v>45743.604166666664</v>
+      </c>
+      <c r="J14">
+        <v>385</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>95291</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15">
+        <v>4875</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J15">
+        <v>55</v>
+      </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>95292</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16">
+        <v>500</v>
+      </c>
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="1">
+        <v>45743.604166666664</v>
+      </c>
+      <c r="J16">
+        <v>940</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>95293</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17">
+        <v>4875</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J17">
+        <v>55</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>95294</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18">
+        <v>4875</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J18">
+        <v>65</v>
+      </c>
+      <c r="K18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>95295</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19">
+        <v>4875</v>
+      </c>
+      <c r="H19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J19">
+        <v>65</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+      <c r="M19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>95296</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20">
+        <v>4875</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J20">
+        <v>72.5</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>95297</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21">
+        <v>4875</v>
+      </c>
+      <c r="H21" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J21">
+        <v>72.5</v>
+      </c>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <v>95298</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22">
+        <v>4875</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J22">
+        <v>77.5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>95299</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23">
+        <v>4875</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="1">
+        <v>45771.604166666664</v>
+      </c>
+      <c r="J23">
+        <v>77.5</v>
+      </c>
+      <c r="K23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
+      <c r="M23" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24">
+        <v>35317</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24">
+        <v>125</v>
+      </c>
+      <c r="H24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="1">
+        <v>45743.604166666664</v>
+      </c>
+      <c r="J24">
+        <v>7500</v>
+      </c>
+      <c r="K24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25">
+        <v>537007</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N25" t="s">
+        <v>82</v>
+      </c>
+      <c r="O25" t="s">
+        <v>83</v>
+      </c>
+      <c r="P25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26">
+        <v>36107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="1">
+        <v>45806.604166666664</v>
+      </c>
+      <c r="J26">
+        <v>27000</v>
+      </c>
+      <c r="K26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="M26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>36108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="1">
+        <v>45806.604166666664</v>
+      </c>
+      <c r="J27">
+        <v>27500</v>
+      </c>
+      <c r="K27" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27">
+        <v>5</v>
+      </c>
+      <c r="M27" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28">
+        <v>36109</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="1">
+        <v>45806.604166666664</v>
+      </c>
+      <c r="J28">
+        <v>27500</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29">
+        <v>119676</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29">
+        <v>150</v>
+      </c>
+      <c r="H29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="1">
+        <v>45743.604166666664</v>
+      </c>
+      <c r="J29">
+        <v>4800</v>
+      </c>
+      <c r="K29" t="s">
+        <v>31</v>
+      </c>
+      <c r="L29">
+        <v>5</v>
+      </c>
+      <c r="M29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30">
+        <v>119677</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30">
+        <v>150</v>
+      </c>
+      <c r="H30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="1">
+        <v>45743.604166666664</v>
+      </c>
+      <c r="J30">
+        <v>4800</v>
+      </c>
+      <c r="K30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30">
+        <v>5</v>
+      </c>
+      <c r="M30" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31">
+        <v>861527</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31">
+        <v>150</v>
+      </c>
+      <c r="H31" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="1">
+        <v>45756.645833333336</v>
+      </c>
+      <c r="J31">
+        <v>4650</v>
+      </c>
+      <c r="K31" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" t="s">
+        <v>46</v>
+      </c>
+      <c r="P31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32">
+        <v>862448</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32">
+        <v>150</v>
+      </c>
+      <c r="H32" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" s="1">
+        <v>45756.645833333336</v>
+      </c>
+      <c r="J32">
+        <v>4800</v>
+      </c>
+      <c r="K32" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+      <c r="M32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" t="s">
+        <v>46</v>
+      </c>
+      <c r="P32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>2013615</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33">
+        <v>150</v>
+      </c>
+      <c r="H33" t="s">
+        <v>102</v>
+      </c>
+      <c r="I33" s="1">
+        <v>45756.645833333336</v>
+      </c>
+      <c r="J33">
+        <v>5100</v>
+      </c>
+      <c r="K33" t="s">
+        <v>34</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="M33" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" t="s">
+        <v>46</v>
+      </c>
+      <c r="P33" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>